<commit_message>
Made changes to script to add Total and highlight Critical
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -14,11 +14,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>NO_Problems</t>
   </si>
   <si>
+    <t>Explanation</t>
+  </si>
+  <si>
+    <t>OC301</t>
+  </si>
+  <si>
+    <t>OC302</t>
+  </si>
+  <si>
     <t>CP001</t>
   </si>
   <si>
@@ -116,13 +125,124 @@
   </si>
   <si>
     <t>OC303</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>No Raritan KVM Specified for the SUT</t>
+  </si>
+  <si>
+    <t>No PDU specified for the SUT</t>
+  </si>
+  <si>
+    <t>No monitoring evidence found in the past 12h for SUT</t>
+  </si>
+  <si>
+    <t>Invalid SUT MAC Address</t>
+  </si>
+  <si>
+    <t>Invalid Program/SKU</t>
+  </si>
+  <si>
+    <t>QDF entry '' must have exactly 4 characters</t>
+  </si>
+  <si>
+    <t>System should be used in VPUX instance 'XXXXX' tag</t>
+  </si>
+  <si>
+    <t>Duplicate Friendly Name</t>
+  </si>
+  <si>
+    <t>No monitoring evidence found in the past 12h for Controller</t>
+  </si>
+  <si>
+    <t>Windows monitoring software for SUT outdated</t>
+  </si>
+  <si>
+    <t>MTL biosfirmware field is invalid</t>
+  </si>
+  <si>
+    <t>Rack or Shelf location is not valid</t>
+  </si>
+  <si>
+    <t>No friendly name found</t>
+  </si>
+  <si>
+    <t>Invalid SUT hostname</t>
+  </si>
+  <si>
+    <t>The system used in VPUX/FW instance doesn't have some tags</t>
+  </si>
+  <si>
+    <t>Invalid SUT IP Address</t>
+  </si>
+  <si>
+    <t>MTL bmcfirmware field is invalid</t>
+  </si>
+  <si>
+    <t>IFWI Information is not set</t>
+  </si>
+  <si>
+    <t>Linux monitoring software for SUT outdated</t>
+  </si>
+  <si>
+    <t>Friendly Name is not valid</t>
+  </si>
+  <si>
+    <t>Duplicate SUT IP Address</t>
+  </si>
+  <si>
+    <t>Missing monitored tag</t>
+  </si>
+  <si>
+    <t>Invalid Controller hostname</t>
+  </si>
+  <si>
+    <t>System 's friendly name is not found in OneCloud</t>
+  </si>
+  <si>
+    <t>Invalid Baseboard Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Instance has status 'Online', but it should be 'Automation'</t>
+  </si>
+  <si>
+    <t>Windows monitoring software for Controller outdated</t>
+  </si>
+  <si>
+    <t>Bios information is not set</t>
+  </si>
+  <si>
+    <t>BKC information is not set</t>
+  </si>
+  <si>
+    <t>Linux monitoring software for Controller outdated</t>
+  </si>
+  <si>
+    <t>Duplicate MAC Address</t>
+  </si>
+  <si>
+    <t>Duplicate NUC Host</t>
+  </si>
+  <si>
+    <t>Duplicate KVM name</t>
+  </si>
+  <si>
+    <t>Invalid Processor Name</t>
+  </si>
+  <si>
+    <t>Invalid NUC Host</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +254,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -174,10 +302,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -219,215 +353,221 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!A2:A36</c:f>
+              <c:f>Sheet1!A2:A35</c:f>
               <c:strCache>
-                <c:ptCount val="35"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
+                  <c:v>OC301</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OC302</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>CP001</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>OC202</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>OC101</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>OC215</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>OC402</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>CJ002</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>CP002</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>CP101</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>OC211</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>OC001</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>CJ001</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>OC403</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>CJ103</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>OC204</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>OC212</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>OC208</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>CP102</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>OC003</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>OC205</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>OC209</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>OC404</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>CJ101</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>OC103</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>CJ102</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>CP103</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>OC206</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>OC207</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>CP104</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>OC203</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>OC304</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>OC214</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>OC104</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>OC303</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!B2:B36</c:f>
+              <c:f>Sheet1!B2:B35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="35"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
+                  <c:v>504</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>423</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>241</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>203</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>155</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>149</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>133</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>108</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>102</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>81</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>79</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>65</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>51</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>48</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>33</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>33</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>31</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -492,215 +632,221 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!A2:A36</c:f>
+              <c:f>Sheet1!A2:A35</c:f>
               <c:strCache>
-                <c:ptCount val="35"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
+                  <c:v>OC301</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OC302</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>CP001</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>OC202</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>OC101</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>OC215</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>OC402</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>CJ002</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>CP002</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>CP101</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>OC211</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>OC001</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>CJ001</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>OC403</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>CJ103</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>OC204</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>OC212</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>OC208</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>CP102</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>OC003</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>OC205</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>OC209</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>OC404</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>CJ101</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>OC103</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>CJ102</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>CP103</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>OC206</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>OC207</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>CP104</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>OC203</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>OC304</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>OC214</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>OC104</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>OC303</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!B2:B36</c:f>
+              <c:f>Sheet1!B2:B35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="35"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
+                  <c:v>504</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>423</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>241</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>203</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>155</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>149</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>133</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>108</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>102</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>81</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>79</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>65</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>51</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>48</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>33</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>33</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>31</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1097,279 +1243,418 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="60.7109375" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:3">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>504</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>423</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
         <v>241</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>203</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>155</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>149</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>133</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>108</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
+        <v>102</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1">
+        <v>81</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1">
+        <v>79</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1">
+        <v>65</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1">
+        <v>51</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1">
+        <v>48</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1">
+        <v>43</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="3" customFormat="1">
+      <c r="A17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="3">
+        <v>36</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="1">
+        <v>34</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="1">
+        <v>33</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1">
+        <v>33</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="1">
+        <v>31</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="3" customFormat="1">
+      <c r="A22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="3">
+        <v>27</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="1">
+        <v>23</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1">
+        <v>23</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="1">
+        <v>18</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="1">
+        <v>14</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="3" customFormat="1">
+      <c r="A27" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="3">
+        <v>13</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="1">
+        <v>9</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="1">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="1">
+        <v>7</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="1">
+        <v>7</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="1">
+        <v>6</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="3" customFormat="1">
+      <c r="A33" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="3">
+        <v>4</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="1">
+        <v>4</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="1">
+        <v>3</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="3" customFormat="1">
+      <c r="A36" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34">
-        <v>2</v>
+      <c r="C36" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="1">
+        <v>2720</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>